<commit_message>
started adding IR update logic
</commit_message>
<xml_diff>
--- a/initial_rosters_with_salary_for_import.xlsx
+++ b/initial_rosters_with_salary_for_import.xlsx
@@ -15,7 +15,7 @@
     <sheet name="initial_rosters_with_salary_for" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">initial_rosters_with_salary_for!$A$1:$J$216</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">initial_rosters_with_salary_for!$A$1:$J$219</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1512,11 +1512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C201" sqref="C201"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8121</v>
       </c>
@@ -1582,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>650</v>
       </c>
@@ -1605,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3214</v>
       </c>
@@ -1628,7 +1627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6845</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8132</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8131</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7591</v>
       </c>
@@ -1720,7 +1719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5846</v>
       </c>
@@ -1743,7 +1742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5967</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5347</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5857</v>
       </c>
@@ -1812,7 +1811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5916</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6783</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6828</v>
       </c>
@@ -1887,7 +1886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>96</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6786</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4018</v>
       </c>
@@ -1956,7 +1955,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4866</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8159</v>
       </c>
@@ -2002,7 +2001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8258</v>
       </c>
@@ -2025,9 +2024,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1067</v>
+        <v>7527</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2039,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1067</v>
+        <v>7527</v>
       </c>
       <c r="F22" t="s">
         <v>44</v>
@@ -2048,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1825</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4951</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7568</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3242</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3199</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6826</v>
       </c>
@@ -2192,7 +2191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6943</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4881</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4035</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>8167</v>
       </c>
@@ -2284,7 +2283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2133</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8129</v>
       </c>
@@ -2330,7 +2329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2449</v>
       </c>
@@ -2353,7 +2352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6790</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1466</v>
       </c>
@@ -2399,7 +2398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7594</v>
       </c>
@@ -2422,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5947</v>
       </c>
@@ -2445,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>367</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2378</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2391</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3163</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8139</v>
       </c>
@@ -2560,7 +2559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>391</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1476</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3664</v>
       </c>
@@ -2629,7 +2628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2309</v>
       </c>
@@ -2658,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1067</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4199</v>
       </c>
@@ -2704,7 +2703,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1386</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5872</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7564</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8112</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1234</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1433</v>
       </c>
@@ -2842,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4149</v>
       </c>
@@ -2865,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>8126</v>
       </c>
@@ -2888,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6814</v>
       </c>
@@ -2911,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6768</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>7601</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>7670</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>6801</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5927</v>
       </c>
@@ -3026,7 +3025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>6151</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>8137</v>
       </c>
@@ -3078,7 +3077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7526</v>
       </c>
@@ -3101,7 +3100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>5185</v>
       </c>
@@ -3124,7 +3123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7561</v>
       </c>
@@ -3147,7 +3146,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>6806</v>
       </c>
@@ -3170,7 +3169,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7553</v>
       </c>
@@ -3193,7 +3192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>6770</v>
       </c>
@@ -3216,7 +3215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>7528</v>
       </c>
@@ -3239,7 +3238,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>8205</v>
       </c>
@@ -3262,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>830</v>
       </c>
@@ -3285,7 +3284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1535</v>
       </c>
@@ -3308,7 +3307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4147</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5122</v>
       </c>
@@ -3354,7 +3353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2306</v>
       </c>
@@ -3377,7 +3376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5248</v>
       </c>
@@ -3403,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>7567</v>
       </c>
@@ -3426,7 +3425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>7571</v>
       </c>
@@ -3449,7 +3448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>6083</v>
       </c>
@@ -3472,7 +3471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>4993</v>
       </c>
@@ -3495,7 +3494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4984</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8135</v>
       </c>
@@ -3541,7 +3540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1339</v>
       </c>
@@ -3564,7 +3563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2197</v>
       </c>
@@ -3587,7 +3586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5850</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5892</v>
       </c>
@@ -3639,7 +3638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4039</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>4040</v>
       </c>
@@ -3685,7 +3684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>8161</v>
       </c>
@@ -3708,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>6951</v>
       </c>
@@ -3731,7 +3730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4892</v>
       </c>
@@ -3754,7 +3753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4981</v>
       </c>
@@ -3777,7 +3776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>4973</v>
       </c>
@@ -3800,7 +3799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>3294</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>7569</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>7839</v>
       </c>
@@ -3875,7 +3874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5001</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5038</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>6955</v>
       </c>
@@ -3947,7 +3946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>7090</v>
       </c>
@@ -3970,7 +3969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>4037</v>
       </c>
@@ -3993,7 +3992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>4988</v>
       </c>
@@ -4016,7 +4015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>7588</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>3321</v>
       </c>
@@ -4062,7 +4061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>5045</v>
       </c>
@@ -4085,7 +4084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>4137</v>
       </c>
@@ -4108,7 +4107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>4034</v>
       </c>
@@ -4131,7 +4130,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>8117</v>
       </c>
@@ -4154,7 +4153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>8221</v>
       </c>
@@ -4177,7 +4176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1426</v>
       </c>
@@ -4206,7 +4205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>6843</v>
       </c>
@@ -4229,7 +4228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>8119</v>
       </c>
@@ -4252,7 +4251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>24</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>4068</v>
       </c>
@@ -4298,7 +4297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>5230</v>
       </c>
@@ -4321,7 +4320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>7547</v>
       </c>
@@ -4344,7 +4343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>3451</v>
       </c>
@@ -4367,7 +4366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1352</v>
       </c>
@@ -4390,7 +4389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2749</v>
       </c>
@@ -4413,7 +4412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>4144</v>
       </c>
@@ -4436,7 +4435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>5848</v>
       </c>
@@ -4459,7 +4458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>7523</v>
       </c>
@@ -4482,7 +4481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>5987</v>
       </c>
@@ -4505,7 +4504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>7543</v>
       </c>
@@ -4528,7 +4527,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>4983</v>
       </c>
@@ -4551,7 +4550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>5849</v>
       </c>
@@ -4580,7 +4579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>4985</v>
       </c>
@@ -4603,7 +4602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>5906</v>
       </c>
@@ -4626,7 +4625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>8142</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>5022</v>
       </c>
@@ -4672,7 +4671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>5890</v>
       </c>
@@ -4695,7 +4694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>6126</v>
       </c>
@@ -4718,7 +4717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>7596</v>
       </c>
@@ -4741,7 +4740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>6945</v>
       </c>
@@ -4764,7 +4763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>4227</v>
       </c>
@@ -4787,7 +4786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>6904</v>
       </c>
@@ -4810,7 +4809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>7538</v>
       </c>
@@ -4833,7 +4832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>8168</v>
       </c>
@@ -4856,7 +4855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>7607</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>8155</v>
       </c>
@@ -4902,7 +4901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2216</v>
       </c>
@@ -4925,7 +4924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>5937</v>
       </c>
@@ -4948,7 +4947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>6813</v>
       </c>
@@ -4971,7 +4970,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>5052</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>17</v>
       </c>
@@ -5017,7 +5016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>5844</v>
       </c>
@@ -5046,7 +5045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2431</v>
       </c>
@@ -5069,7 +5068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>3225</v>
       </c>
@@ -5092,7 +5091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>5095</v>
       </c>
@@ -5115,7 +5114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>5110</v>
       </c>
@@ -5138,7 +5137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>8154</v>
       </c>
@@ -5164,7 +5163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>4217</v>
       </c>
@@ -5187,7 +5186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>4663</v>
       </c>
@@ -5210,7 +5209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>8118</v>
       </c>
@@ -5233,7 +5232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>8144</v>
       </c>
@@ -5256,7 +5255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>167</v>
       </c>
@@ -5279,7 +5278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>7610</v>
       </c>
@@ -5302,7 +5301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>4017</v>
       </c>
@@ -5325,7 +5324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1166</v>
       </c>
@@ -5348,7 +5347,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>6794</v>
       </c>
@@ -5371,7 +5370,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>3969</v>
       </c>
@@ -5394,7 +5393,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>4029</v>
       </c>
@@ -5417,7 +5416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>956</v>
       </c>
@@ -5446,7 +5445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>3202</v>
       </c>
@@ -5469,7 +5468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>3976</v>
       </c>
@@ -5492,7 +5491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>4082</v>
       </c>
@@ -5515,7 +5514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>8211</v>
       </c>
@@ -5538,7 +5537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1945</v>
       </c>
@@ -5561,7 +5560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>3423</v>
       </c>
@@ -5584,7 +5583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>5917</v>
       </c>
@@ -5607,7 +5606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>5955</v>
       </c>
@@ -5630,7 +5629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1264</v>
       </c>
@@ -5653,7 +5652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>421</v>
       </c>
@@ -5676,7 +5675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>4098</v>
       </c>
@@ -5699,7 +5698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1049</v>
       </c>
@@ -5722,7 +5721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>4033</v>
       </c>
@@ -5745,7 +5744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>1479</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>3271</v>
       </c>
@@ -5791,7 +5790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2374</v>
       </c>
@@ -5814,7 +5813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>2320</v>
       </c>
@@ -5837,7 +5836,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>947</v>
       </c>
@@ -5866,7 +5865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>6694</v>
       </c>
@@ -5889,7 +5888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>6804</v>
       </c>
@@ -5912,7 +5911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>7606</v>
       </c>
@@ -5935,7 +5934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>7608</v>
       </c>
@@ -5958,7 +5957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>8130</v>
       </c>
@@ -5981,7 +5980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>8153</v>
       </c>
@@ -6004,7 +6003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>7600</v>
       </c>
@@ -6027,7 +6026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>2028</v>
       </c>
@@ -6050,7 +6049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>1992</v>
       </c>
@@ -6073,7 +6072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>4046</v>
       </c>
@@ -6096,7 +6095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1689</v>
       </c>
@@ -6119,7 +6118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>7525</v>
       </c>
@@ -6142,7 +6141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>6819</v>
       </c>
@@ -6165,7 +6164,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>8151</v>
       </c>
@@ -6188,7 +6187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>3164</v>
       </c>
@@ -6658,12 +6657,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J216">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="12"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:J219">
     <sortState ref="A201:J216">
       <sortCondition ref="G1:G216"/>
     </sortState>

</xml_diff>